<commit_message>
update application with module files
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_NardouThomas.xlsx
+++ b/Journal-de-Travail_NardouThomas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pk88yte\Documents\GitHub\P_Security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96B91CC-B553-4FBC-8B5B-4FC1340D5BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767FB10C-23DB-446A-BD1C-9CD12C814B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>J'ai reflechis à ce que je pouvais rajouter comme maquette en plus de celles que j'avais fais mais sans résultat la prochain je continurai mais si au bout de 15 min je trouve rien je m'arreterais là</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai discuté avec M. Schaffter pour qu'il m'explique desbout de code qu'il nous avait fournis </t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1072,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -2000,7 +2003,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2053,7 +2056,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 1 heurs 45 minutes</v>
+        <v>0 jours 2 heurs 0 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2072,11 +2075,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2305,15 +2308,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="str">
+      <c r="A14" s="8">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="47"/>
+        <v>16</v>
+      </c>
+      <c r="B14" s="47">
+        <v>45401</v>
+      </c>
       <c r="C14" s="48"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="37"/>
+      <c r="D14" s="49">
+        <v>15</v>
+      </c>
+      <c r="E14" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>36</v>
+      </c>
       <c r="G14" s="16"/>
       <c r="M14" t="s">
         <v>21</v>
@@ -8669,7 +8680,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8677,7 +8688,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8786,7 +8797,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>7.2916666666666671E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9023,6 +9034,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9031,15 +9051,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9062,6 +9073,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9070,12 +9089,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add get user infos routes
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_NardouThomas.xlsx
+++ b/Journal-de-Travail_NardouThomas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pk88yte\Documents\GitHub\P_Security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E06B38-0845-4214-84E0-DB789398FC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FB9A52-249C-4741-AB1E-EFB194EED761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -167,6 +167,18 @@
   </si>
   <si>
     <t xml:space="preserve">J'ai hashé le password et j'envoie les informations dans la base de donnée </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai regler un problème lors de la connection de l'utilisateur </t>
+  </si>
+  <si>
+    <t>J'ai finalisé la requête pour obtenir ses information avec un système de vérification des permissions</t>
+  </si>
+  <si>
+    <t>J'ai regler quelque petits problème encore en lien avec l'obtention avec ses informations et j'ai aidé lucas a regler un soucis avec node JS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai installé le package cookies-parser pour pouvoir stocker le tocker de l'utilisateur si j'ai pris autant de temps c'est parce que j'avais eu un problème d'installation </t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1099,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.2916666666666671E-2</c:v>
+                  <c:v>0.12152777777777778</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -2018,7 +2030,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2071,7 +2083,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 3 heurs 30 minutes</v>
+        <v>0 jours 4 heurs 40 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2090,11 +2102,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>210</v>
+        <v>280</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>210</v>
+        <v>280</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2479,45 +2491,69 @@
       </c>
       <c r="B20" s="47"/>
       <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="37"/>
+      <c r="D20" s="49">
+        <v>20</v>
+      </c>
+      <c r="E20" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>42</v>
+      </c>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="str">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
         <v/>
       </c>
       <c r="B21" s="51"/>
       <c r="C21" s="52"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="37"/>
+      <c r="D21" s="53">
+        <v>15</v>
+      </c>
+      <c r="E21" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>43</v>
+      </c>
       <c r="G21" s="18"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="str">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
         <v/>
       </c>
       <c r="B22" s="47"/>
       <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="37"/>
+      <c r="D22" s="49">
+        <v>15</v>
+      </c>
+      <c r="E22" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>44</v>
+      </c>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="str">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
         <v/>
       </c>
       <c r="B23" s="51"/>
       <c r="C23" s="52"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="37"/>
+      <c r="D23" s="53">
+        <v>20</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>45</v>
+      </c>
       <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -8735,7 +8771,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8743,7 +8779,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>7.2916666666666671E-2</v>
+        <v>0.12152777777777778</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8852,7 +8888,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.14583333333333334</v>
+        <v>0.19444444444444442</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9089,6 +9125,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9097,15 +9142,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9128,6 +9164,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9136,12 +9180,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add cookies system and add login system in front
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_NardouThomas.xlsx
+++ b/Journal-de-Travail_NardouThomas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pk88yte\Documents\GitHub\P_Security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FB9A52-249C-4741-AB1E-EFB194EED761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E2D220-3939-415B-820D-75C56399001F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -179,6 +179,21 @@
   </si>
   <si>
     <t xml:space="preserve">J'ai installé le package cookies-parser pour pouvoir stocker le tocker de l'utilisateur si j'ai pris autant de temps c'est parce que j'avais eu un problème d'installation </t>
+  </si>
+  <si>
+    <t>J'ai mis mes différentes application en https que ce soit le frontend ou le backend</t>
+  </si>
+  <si>
+    <t>J'ai regarder les fonctionnalité demandé dans le cahier des charges est regardé ce que j'avais fais ou pas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai créer une page de login et j'essaie actuellement de stocker le token dans les cookies </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai réussi a stocker le token de l'utilisateur mais je n'arrive pas à le récuperrer </t>
+  </si>
+  <si>
+    <t>J'ai terminer ma page de login et mes routes de l'utilisateur</t>
   </si>
 </sst>
 </file>
@@ -1099,13 +1114,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.12152777777777778</c:v>
+                  <c:v>0.19791666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0416666666666666E-2</c:v>
+                  <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2030,7 +2045,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2083,7 +2098,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 4 heurs 40 minutes</v>
+        <v>0 jours 6 heurs 45 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2102,11 +2117,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>280</v>
+        <v>405</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>280</v>
+        <v>405</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2485,11 +2500,13 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="str">
+      <c r="A20" s="8">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="47"/>
+        <v>4</v>
+      </c>
+      <c r="B20" s="47">
+        <v>26.24</v>
+      </c>
       <c r="C20" s="48"/>
       <c r="D20" s="49">
         <v>20</v>
@@ -2503,11 +2520,13 @@
       <c r="G20" s="16"/>
     </row>
     <row r="21" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="str">
+      <c r="A21" s="17">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="51"/>
+        <v>17</v>
+      </c>
+      <c r="B21" s="51">
+        <v>45408</v>
+      </c>
       <c r="C21" s="52"/>
       <c r="D21" s="53">
         <v>15</v>
@@ -2521,11 +2540,13 @@
       <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="str">
+      <c r="A22" s="8">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="47"/>
+        <v>17</v>
+      </c>
+      <c r="B22" s="47">
+        <v>45408</v>
+      </c>
       <c r="C22" s="48"/>
       <c r="D22" s="49">
         <v>15</v>
@@ -2539,11 +2560,13 @@
       <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="str">
+      <c r="A23" s="17">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="51"/>
+        <v>17</v>
+      </c>
+      <c r="B23" s="51">
+        <v>45408</v>
+      </c>
       <c r="C23" s="52"/>
       <c r="D23" s="53">
         <v>20</v>
@@ -2557,27 +2580,41 @@
       <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="str">
+      <c r="A24" s="8">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="47"/>
+        <v>18</v>
+      </c>
+      <c r="B24" s="47">
+        <v>45415</v>
+      </c>
       <c r="C24" s="48"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="37"/>
+      <c r="D24" s="49">
+        <v>25</v>
+      </c>
+      <c r="E24" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>46</v>
+      </c>
       <c r="G24" s="16"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="str">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
         <v/>
       </c>
       <c r="B25" s="51"/>
       <c r="C25" s="52"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="37"/>
+      <c r="D25" s="53">
+        <v>15</v>
+      </c>
+      <c r="E25" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>47</v>
+      </c>
       <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2587,9 +2624,15 @@
       </c>
       <c r="B26" s="47"/>
       <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="37"/>
+      <c r="D26" s="49">
+        <v>30</v>
+      </c>
+      <c r="E26" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>48</v>
+      </c>
       <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2599,9 +2642,15 @@
       </c>
       <c r="B27" s="51"/>
       <c r="C27" s="52"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="37"/>
+      <c r="D27" s="53">
+        <v>25</v>
+      </c>
+      <c r="E27" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>49</v>
+      </c>
       <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2611,9 +2660,15 @@
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="48"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="36"/>
+      <c r="D28" s="49">
+        <v>30</v>
+      </c>
+      <c r="E28" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>50</v>
+      </c>
       <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -8771,7 +8826,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>175</v>
+        <v>285</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8779,7 +8834,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.12152777777777778</v>
+        <v>0.19791666666666666</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8807,7 +8862,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C7" s="28" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8815,7 +8870,7 @@
       </c>
       <c r="D7" s="34">
         <f t="shared" si="0"/>
-        <v>1.0416666666666666E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8888,7 +8943,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.19444444444444442</v>
+        <v>0.28125</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9125,15 +9180,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9142,6 +9188,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9164,14 +9219,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9180,4 +9227,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
finish and validate the project
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_NardouThomas.xlsx
+++ b/Journal-de-Travail_NardouThomas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pk88yte\Documents\GitHub\P_Security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E2D220-3939-415B-820D-75C56399001F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6ED8F4B-518E-4EB5-9A10-804197418A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>J'ai terminer ma page de login et mes routes de l'utilisateur</t>
+  </si>
+  <si>
+    <t>J'ai terminé ma route pour les administrateur et j'ai paufiner les dernier détails</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1117,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19791666666666666</c:v>
+                  <c:v>0.21180555555555555</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -2045,7 +2048,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2098,7 +2101,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 6 heurs 45 minutes</v>
+        <v>0 jours 7 heurs 5 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2117,11 +2120,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>405</v>
+        <v>425</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>405</v>
+        <v>425</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2600,11 +2603,13 @@
       <c r="G24" s="16"/>
     </row>
     <row r="25" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="str">
+      <c r="A25" s="17">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="51"/>
+        <v>18</v>
+      </c>
+      <c r="B25" s="51">
+        <v>45415</v>
+      </c>
       <c r="C25" s="52"/>
       <c r="D25" s="53">
         <v>15</v>
@@ -2618,11 +2623,13 @@
       <c r="G25" s="18"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="str">
+      <c r="A26" s="8">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="47"/>
+        <v>18</v>
+      </c>
+      <c r="B26" s="47">
+        <v>45415</v>
+      </c>
       <c r="C26" s="48"/>
       <c r="D26" s="49">
         <v>30</v>
@@ -2636,11 +2643,13 @@
       <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="str">
+      <c r="A27" s="17">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="51"/>
+        <v>18</v>
+      </c>
+      <c r="B27" s="51">
+        <v>45415</v>
+      </c>
       <c r="C27" s="52"/>
       <c r="D27" s="53">
         <v>25</v>
@@ -2654,11 +2663,13 @@
       <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="str">
+      <c r="A28" s="8">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="47"/>
+        <v>18</v>
+      </c>
+      <c r="B28" s="47">
+        <v>45415</v>
+      </c>
       <c r="C28" s="48"/>
       <c r="D28" s="49">
         <v>30</v>
@@ -2672,15 +2683,23 @@
       <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="str">
+      <c r="A29" s="17">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="51"/>
+        <v>20</v>
+      </c>
+      <c r="B29" s="51">
+        <v>45429</v>
+      </c>
       <c r="C29" s="52"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="36"/>
+      <c r="D29" s="53">
+        <v>20</v>
+      </c>
+      <c r="E29" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="36" t="s">
+        <v>51</v>
+      </c>
       <c r="G29" s="18"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -8826,7 +8845,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>285</v>
+        <v>305</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8834,7 +8853,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.19791666666666666</v>
+        <v>0.21180555555555555</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8943,7 +8962,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.28125</v>
+        <v>0.2951388888888889</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9180,6 +9199,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9188,15 +9216,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9219,6 +9238,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9227,12 +9254,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>